<commit_message>
Adjusted FunctionalOrMentalStatus mapping Excel file
</commit_message>
<xml_diff>
--- a/Supporting documents/FunctionalOrMentalStatus.xlsx
+++ b/Supporting documents/FunctionalOrMentalStatus.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -90,9 +90,6 @@
     <t>StatusDate</t>
   </si>
   <si>
-    <t>Observation.component.valueCodeableConcept</t>
-  </si>
-  <si>
     <t>StatusNaamICFCodelijst</t>
   </si>
   <si>
@@ -177,35 +174,9 @@
     <t>Valueset OID 2.16.840.1.113883.2.4.3.11.60.40.2.4.26.8</t>
   </si>
   <si>
-    <t>Terminology binding not avaiblable in the ZIB. Need to add valueset binding</t>
-  </si>
-  <si>
-    <t>Terminology binding not avaiblable in the ZIB Need to add valueset binding</t>
-  </si>
-  <si>
     <t>Fits</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Why is this even in the ZIB? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Have to put an Extension.</t>
-    </r>
-  </si>
-  <si>
-    <t> ZIB-570</t>
-  </si>
-  <si>
-    <t>Created a BITS issue for Terminology</t>
-  </si>
-  <si>
     <t>STU3</t>
   </si>
   <si>
@@ -216,6 +187,18 @@
   </si>
   <si>
     <t>Set constrains on references to  only ZIB profiles for new basedOn element and context element in the nl-core-observation</t>
+  </si>
+  <si>
+    <t>Observation.code</t>
+  </si>
+  <si>
+    <t>Observation.valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>Have to put an Extension.</t>
+  </si>
+  <si>
+    <t>Need to put a constraint that covers the following:If both the status name and the status value are recorded in code, then both values must come from the same code system. If the patient uses a medical aid, the evaluation of the extent of the limitation will take place without this aid.</t>
   </si>
 </sst>
 </file>
@@ -513,7 +496,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -595,40 +578,41 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -935,7 +919,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -955,15 +939,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -976,22 +960,22 @@
     </row>
     <row r="2" spans="1:12" ht="15">
       <c r="A2" s="3"/>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="25.5">
+    <row r="3" spans="1:12" ht="63.75">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1010,13 +994,13 @@
         <v>9</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="25.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -1035,21 +1019,19 @@
         <v>10</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>54</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
         <v>23</v>
@@ -1063,7 +1045,7 @@
         <v>13</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1071,10 +1053,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
         <v>6</v>
@@ -1088,7 +1070,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15">
@@ -1096,10 +1078,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18" t="s">
         <v>20</v>
@@ -1112,46 +1094,41 @@
       <c r="J7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="24" t="s">
-        <v>56</v>
+      <c r="K7" s="41" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="K9" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="28" t="s">
-        <v>57</v>
-      </c>
+      <c r="L9" s="28"/>
     </row>
     <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
+      <c r="A13" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1164,16 +1141,16 @@
     </row>
     <row r="15" spans="1:12" ht="15">
       <c r="A15" s="3"/>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="38"/>
       <c r="J15" s="4" t="s">
         <v>5</v>
       </c>
@@ -1198,7 +1175,7 @@
         <v>9</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="K16" s="27"/>
     </row>
@@ -1221,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="K17" s="27"/>
     </row>
@@ -1230,10 +1207,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="36"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12" t="s">
         <v>23</v>
@@ -1253,10 +1230,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12" t="s">
         <v>6</v>
@@ -1266,8 +1243,8 @@
       <c r="I19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="39" t="s">
-        <v>60</v>
+      <c r="J19" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="K19" s="26"/>
     </row>
@@ -1276,10 +1253,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="17"/>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="29"/>
+      <c r="D20" s="40"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18" t="s">
         <v>20</v>
@@ -1295,34 +1272,31 @@
       <c r="K20" s="24"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="B22" s="40" t="s">
-        <v>61</v>
+      <c r="B22" s="30" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="B23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="L9" r:id="rId1" display="https://bits.nictiz.nl/browse/ZIB-570"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1343,130 +1317,130 @@
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
         <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>28</v>
-      </c>
-      <c r="D21" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
         <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>28</v>
-      </c>
-      <c r="D28" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
         <v>43</v>
-      </c>
-      <c r="D29" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1491,130 +1465,130 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>28</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
         <v>27</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>28</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
         <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>